<commit_message>
2.1.2: Enable class annotation and import list.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoResourceBundleBundleStructure.xlsx
+++ b/meta/program/BlancoResourceBundleBundleStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoResourceBundle/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DD5A216-DFDD-DE49-BC13-EBCD2C407A8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EF323C-8EF5-E74A-A99C-9C2DF3B94D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,15 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="92512"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -284,12 +287,57 @@
     <t>new java.util.ArrayList&lt;blanco.resourcebundle.valueobject.BlancoResourceBundleBundleItemStructure&gt;()</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>annotationList</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>java.util.List&lt;java.lang.String&gt;</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>new java.util.ArrayList&lt;java.lang.String&gt;()</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>クラスのアノテーションを指定します。</t>
+    <rPh sb="12" eb="14">
+      <t>シテイシマス。</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>importList</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>importを指定します。</t>
+    <rPh sb="7" eb="9">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>annotation</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ワークに利用されるフィールド。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ワークニリヨウサレル </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -312,6 +360,18 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -679,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -792,6 +852,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -801,17 +880,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1126,13 +1196,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -1286,14 +1358,14 @@
       <c r="D16" s="16"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1303,27 +1375,27 @@
       <c r="E18" s="6"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="44" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="50"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="49"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="50"/>
+    <row r="20" spans="1:7">
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="49"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="18"/>
       <c r="B21" s="20"/>
       <c r="C21" s="27"/>
@@ -1331,7 +1403,7 @@
       <c r="E21" s="37"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="22"/>
       <c r="B22" s="24"/>
       <c r="C22" s="28"/>
@@ -1339,14 +1411,14 @@
       <c r="E22" s="38"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
@@ -1356,33 +1428,33 @@
       <c r="E24" s="8"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="44" t="s">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A25" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="50" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="26"/>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
+    <row r="26" spans="1:7">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="18">
         <v>1</v>
       </c>
@@ -1398,8 +1470,9 @@
       </c>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="1:6" ht="27.5" customHeight="1">
+    <row r="28" spans="1:7" ht="27.5" customHeight="1">
       <c r="A28" s="40">
+        <f>A27+1</f>
         <v>2</v>
       </c>
       <c r="B28" s="41" t="s">
@@ -1411,13 +1484,14 @@
       <c r="D28" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="49"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="F28" s="48"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="40">
+        <f t="shared" ref="A29:A40" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="41" t="s">
@@ -1432,8 +1506,9 @@
       </c>
       <c r="F29" s="43"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="40">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B30" s="41" t="s">
@@ -1448,128 +1523,194 @@
       </c>
       <c r="F30" s="43"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7" s="46" customFormat="1" ht="45">
       <c r="A31" s="40">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="43"/>
-    </row>
-    <row r="32" spans="1:6" ht="28.25" customHeight="1">
+      <c r="B31" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="48"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" s="46" customFormat="1" ht="45">
       <c r="A32" s="40">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B32" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="49"/>
+      <c r="B32" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="48"/>
+      <c r="G32"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="40">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>60</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D33" s="42"/>
       <c r="E33" s="42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F33" s="43"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="28.25" customHeight="1">
       <c r="A34" s="40">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
+      <c r="B34" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="48"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="40">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>60</v>
+      </c>
       <c r="E35" s="42" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F35" s="43"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="40">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B36" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>35</v>
-      </c>
+      <c r="B36" s="41"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="42"/>
-      <c r="E36" s="42" t="s">
-        <v>53</v>
-      </c>
+      <c r="E36" s="42"/>
       <c r="F36" s="43"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="40">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D37" s="42"/>
       <c r="E37" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="40">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="40">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="43"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="25"/>
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="40">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="43"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="22"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="A19:A20"/>
@@ -1580,26 +1721,28 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D54">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D57" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1612,7 +1755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>